<commit_message>
Update the Amazon statement upload feature on the Order Analysis page
</commit_message>
<xml_diff>
--- a/app/Ref/stock.xlsx
+++ b/app/Ref/stock.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sionp\Work\Dev\nextjs\order-dash\app\Ref\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E91193D-F045-446E-AFDB-E652EF14E9BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9584A85-B76E-41B0-8792-D48F2A0F317D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="11475" xr2:uid="{0DA9C929-26C5-498E-A021-041CA548DA6F}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$E$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$E$1789</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -11291,7 +11291,7 @@
   <dimension ref="A1:E1789"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.649999999999999"/>
@@ -11327,10 +11327,10 @@
         <v>1</v>
       </c>
       <c r="C2" s="1">
-        <v>303</v>
+        <v>297</v>
       </c>
       <c r="D2" s="1">
-        <v>173</v>
+        <v>158</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -11355,10 +11355,10 @@
         <v>5</v>
       </c>
       <c r="C4" s="1">
-        <v>400</v>
+        <v>388</v>
       </c>
       <c r="D4" s="1">
-        <v>72</v>
+        <v>62</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -11369,10 +11369,10 @@
         <v>7</v>
       </c>
       <c r="C5" s="1">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="D5" s="1">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -11383,10 +11383,10 @@
         <v>9</v>
       </c>
       <c r="C6" s="1">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="D6" s="1">
-        <v>61</v>
+        <v>51</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -11397,10 +11397,10 @@
         <v>11</v>
       </c>
       <c r="C7" s="1">
-        <v>106</v>
+        <v>84</v>
       </c>
       <c r="D7" s="1">
-        <v>317</v>
+        <v>229</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -11414,7 +11414,7 @@
         <v>39</v>
       </c>
       <c r="D8" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -11425,10 +11425,10 @@
         <v>15</v>
       </c>
       <c r="C9" s="1">
-        <v>130</v>
+        <v>68</v>
       </c>
       <c r="D9" s="1">
-        <v>93</v>
+        <v>68</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -11439,10 +11439,10 @@
         <v>17</v>
       </c>
       <c r="C10" s="1">
-        <v>229</v>
+        <v>196</v>
       </c>
       <c r="D10" s="1">
-        <v>65</v>
+        <v>53</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -11453,7 +11453,7 @@
         <v>19</v>
       </c>
       <c r="C11" s="1">
-        <v>100</v>
+        <v>87</v>
       </c>
       <c r="D11" s="1">
         <v>6</v>
@@ -11481,7 +11481,7 @@
         <v>23</v>
       </c>
       <c r="C13" s="1">
-        <v>51</v>
+        <v>34</v>
       </c>
       <c r="D13" s="1">
         <v>0</v>
@@ -11523,7 +11523,7 @@
         <v>29</v>
       </c>
       <c r="C16" s="1">
-        <v>217</v>
+        <v>210</v>
       </c>
       <c r="D16" s="1">
         <v>24</v>
@@ -11537,7 +11537,7 @@
         <v>31</v>
       </c>
       <c r="C17" s="2">
-        <v>80</v>
+        <v>238</v>
       </c>
       <c r="D17" s="2">
         <v>0</v>
@@ -11551,7 +11551,7 @@
         <v>33</v>
       </c>
       <c r="C18" s="2">
-        <v>154</v>
+        <v>142</v>
       </c>
       <c r="D18" s="2">
         <v>0</v>
@@ -11579,7 +11579,7 @@
         <v>37</v>
       </c>
       <c r="C20" s="2">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D20" s="2">
         <v>0</v>
@@ -11621,7 +11621,7 @@
         <v>43</v>
       </c>
       <c r="C23" s="1">
-        <v>209</v>
+        <v>165</v>
       </c>
       <c r="D23" s="1">
         <v>0</v>
@@ -11649,7 +11649,7 @@
         <v>47</v>
       </c>
       <c r="C25" s="1">
-        <v>4</v>
+        <v>-4</v>
       </c>
       <c r="D25" s="1">
         <v>0</v>
@@ -11691,7 +11691,7 @@
         <v>53</v>
       </c>
       <c r="C28" s="1">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="D28" s="1">
         <v>0</v>
@@ -11719,7 +11719,7 @@
         <v>57</v>
       </c>
       <c r="C30" s="1">
-        <v>65</v>
+        <v>30</v>
       </c>
       <c r="D30" s="1">
         <v>0</v>
@@ -11733,7 +11733,7 @@
         <v>59</v>
       </c>
       <c r="C31" s="1">
-        <v>22</v>
+        <v>55</v>
       </c>
       <c r="D31" s="1">
         <v>0</v>
@@ -11747,7 +11747,7 @@
         <v>61</v>
       </c>
       <c r="C32" s="1">
-        <v>19</v>
+        <v>161</v>
       </c>
       <c r="D32" s="1">
         <v>0</v>
@@ -11761,7 +11761,7 @@
         <v>63</v>
       </c>
       <c r="C33" s="1">
-        <v>76</v>
+        <v>63</v>
       </c>
       <c r="D33" s="1">
         <v>0</v>
@@ -11789,7 +11789,7 @@
         <v>67</v>
       </c>
       <c r="C35" s="1">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D35" s="1">
         <v>0</v>
@@ -11803,7 +11803,7 @@
         <v>69</v>
       </c>
       <c r="C36" s="1">
-        <v>53</v>
+        <v>41</v>
       </c>
       <c r="D36" s="1">
         <v>0</v>
@@ -11817,7 +11817,7 @@
         <v>71</v>
       </c>
       <c r="C37" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D37" s="1">
         <v>0</v>
@@ -11831,7 +11831,7 @@
         <v>73</v>
       </c>
       <c r="C38" s="1">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D38" s="1">
         <v>0</v>
@@ -11845,7 +11845,7 @@
         <v>75</v>
       </c>
       <c r="C39" s="1">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="D39" s="1">
         <v>0</v>
@@ -11859,7 +11859,7 @@
         <v>77</v>
       </c>
       <c r="C40" s="1">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="D40" s="1">
         <v>0</v>
@@ -11873,7 +11873,7 @@
         <v>79</v>
       </c>
       <c r="C41" s="1">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D41" s="1">
         <v>0</v>
@@ -11887,7 +11887,7 @@
         <v>81</v>
       </c>
       <c r="C42" s="1">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D42" s="1">
         <v>0</v>
@@ -11901,7 +11901,7 @@
         <v>83</v>
       </c>
       <c r="C43" s="1">
-        <v>22</v>
+        <v>2</v>
       </c>
       <c r="D43" s="1">
         <v>0</v>
@@ -11915,7 +11915,7 @@
         <v>85</v>
       </c>
       <c r="C44" s="1">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D44" s="1">
         <v>0</v>
@@ -11943,7 +11943,7 @@
         <v>89</v>
       </c>
       <c r="C46" s="1">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="D46" s="1">
         <v>0</v>
@@ -11957,7 +11957,7 @@
         <v>91</v>
       </c>
       <c r="C47" s="1">
-        <v>162</v>
+        <v>148</v>
       </c>
       <c r="D47" s="1">
         <v>0</v>
@@ -11971,7 +11971,7 @@
         <v>93</v>
       </c>
       <c r="C48" s="1">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="D48" s="1">
         <v>0</v>
@@ -11985,7 +11985,7 @@
         <v>95</v>
       </c>
       <c r="C49" s="1">
-        <v>224</v>
+        <v>128</v>
       </c>
       <c r="D49" s="1">
         <v>0</v>
@@ -12013,7 +12013,7 @@
         <v>99</v>
       </c>
       <c r="C51" s="1">
-        <v>34</v>
+        <v>390</v>
       </c>
       <c r="D51" s="1">
         <v>0</v>
@@ -12027,7 +12027,7 @@
         <v>101</v>
       </c>
       <c r="C52" s="1">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D52" s="1">
         <v>0</v>
@@ -12041,7 +12041,7 @@
         <v>103</v>
       </c>
       <c r="C53" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D53" s="1">
         <v>0</v>
@@ -12055,7 +12055,7 @@
         <v>105</v>
       </c>
       <c r="C54" s="5">
-        <v>3552</v>
+        <v>3411</v>
       </c>
       <c r="D54" s="1">
         <v>0</v>
@@ -12069,7 +12069,7 @@
         <v>107</v>
       </c>
       <c r="C55" s="1">
-        <v>4</v>
+        <v>50</v>
       </c>
       <c r="D55" s="1">
         <v>0</v>
@@ -12097,7 +12097,7 @@
         <v>111</v>
       </c>
       <c r="C57" s="1">
-        <v>414</v>
+        <v>379</v>
       </c>
       <c r="D57" s="1">
         <v>0</v>
@@ -12139,7 +12139,7 @@
         <v>117</v>
       </c>
       <c r="C60" s="1">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="D60" s="1">
         <v>0</v>
@@ -12167,7 +12167,7 @@
         <v>121</v>
       </c>
       <c r="C62" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D62" s="1">
         <v>0</v>
@@ -12181,7 +12181,7 @@
         <v>123</v>
       </c>
       <c r="C63" s="1">
-        <v>205</v>
+        <v>163</v>
       </c>
       <c r="D63" s="1">
         <v>0</v>
@@ -12209,7 +12209,7 @@
         <v>127</v>
       </c>
       <c r="C65" s="1">
-        <v>498</v>
+        <v>495</v>
       </c>
       <c r="D65" s="1">
         <v>0</v>
@@ -12237,7 +12237,7 @@
         <v>131</v>
       </c>
       <c r="C67" s="1">
-        <v>682</v>
+        <v>652</v>
       </c>
       <c r="D67" s="1">
         <v>0</v>
@@ -12251,7 +12251,7 @@
         <v>133</v>
       </c>
       <c r="C68" s="1">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="D68" s="1">
         <v>0</v>
@@ -12265,7 +12265,7 @@
         <v>135</v>
       </c>
       <c r="C69" s="1">
-        <v>145</v>
+        <v>127</v>
       </c>
       <c r="D69" s="1">
         <v>0</v>
@@ -12279,7 +12279,7 @@
         <v>137</v>
       </c>
       <c r="C70" s="1">
-        <v>139</v>
+        <v>132</v>
       </c>
       <c r="D70" s="1">
         <v>0</v>
@@ -12307,7 +12307,7 @@
         <v>141</v>
       </c>
       <c r="C72" s="1">
-        <v>35</v>
+        <v>14</v>
       </c>
       <c r="D72" s="1">
         <v>0</v>
@@ -12321,7 +12321,7 @@
         <v>143</v>
       </c>
       <c r="C73" s="1">
-        <v>341</v>
+        <v>286</v>
       </c>
       <c r="D73" s="1">
         <v>0</v>
@@ -12335,7 +12335,7 @@
         <v>145</v>
       </c>
       <c r="C74" s="1">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="D74" s="1">
         <v>0</v>
@@ -12349,7 +12349,7 @@
         <v>147</v>
       </c>
       <c r="C75" s="1">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="D75" s="1">
         <v>0</v>
@@ -12363,7 +12363,7 @@
         <v>149</v>
       </c>
       <c r="C76" s="1">
-        <v>99</v>
+        <v>51</v>
       </c>
       <c r="D76" s="1">
         <v>0</v>
@@ -12391,7 +12391,7 @@
         <v>153</v>
       </c>
       <c r="C78" s="1">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="D78" s="1">
         <v>0</v>
@@ -12447,7 +12447,7 @@
         <v>161</v>
       </c>
       <c r="C82" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D82" s="1">
         <v>0</v>
@@ -12464,7 +12464,7 @@
         <v>0</v>
       </c>
       <c r="D83" s="1">
-        <v>139</v>
+        <v>113</v>
       </c>
     </row>
     <row r="84" spans="1:4">
@@ -12478,7 +12478,7 @@
         <v>0</v>
       </c>
       <c r="D84" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="85" spans="1:4">
@@ -12530,7 +12530,7 @@
         <v>0</v>
       </c>
       <c r="D88" s="1">
-        <v>30</v>
+        <v>24</v>
       </c>
     </row>
     <row r="89" spans="1:4">
@@ -12558,7 +12558,7 @@
         <v>0</v>
       </c>
       <c r="D90" s="1">
-        <v>17</v>
+        <v>5</v>
       </c>
     </row>
     <row r="91" spans="1:4">
@@ -12572,7 +12572,7 @@
         <v>0</v>
       </c>
       <c r="D91" s="1">
-        <v>9</v>
+        <v>1</v>
       </c>
     </row>
     <row r="92" spans="1:4">
@@ -12586,7 +12586,7 @@
         <v>6</v>
       </c>
       <c r="D92" s="1">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="93" spans="1:4">
@@ -12597,7 +12597,7 @@
         <v>181</v>
       </c>
       <c r="C93" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D93" s="1">
         <v>0</v>
@@ -12614,7 +12614,7 @@
         <v>0</v>
       </c>
       <c r="D94" s="1">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="95" spans="1:4">
@@ -12698,7 +12698,7 @@
         <v>7</v>
       </c>
       <c r="D100" s="1">
-        <v>13</v>
+        <v>9</v>
       </c>
     </row>
     <row r="101" spans="1:4">
@@ -12819,7 +12819,7 @@
         <v>207</v>
       </c>
       <c r="C110" s="1">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D110" s="1">
         <v>0</v>
@@ -12847,7 +12847,7 @@
         <v>211</v>
       </c>
       <c r="C112" s="1">
-        <v>592</v>
+        <v>577</v>
       </c>
       <c r="D112" s="1">
         <v>0</v>
@@ -12861,7 +12861,7 @@
         <v>213</v>
       </c>
       <c r="C113" s="1">
-        <v>253</v>
+        <v>220</v>
       </c>
       <c r="D113" s="1">
         <v>0</v>
@@ -12875,7 +12875,7 @@
         <v>215</v>
       </c>
       <c r="C114" s="1">
-        <v>36</v>
+        <v>9</v>
       </c>
       <c r="D114" s="1">
         <v>0</v>
@@ -12903,7 +12903,7 @@
         <v>219</v>
       </c>
       <c r="C116" s="1">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="D116" s="1">
         <v>0</v>
@@ -12931,7 +12931,7 @@
         <v>223</v>
       </c>
       <c r="C118" s="1">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D118" s="1">
         <v>0</v>
@@ -12945,7 +12945,7 @@
         <v>225</v>
       </c>
       <c r="C119" s="1">
-        <v>40</v>
+        <v>342</v>
       </c>
       <c r="D119" s="1">
         <v>0</v>
@@ -12959,7 +12959,7 @@
         <v>227</v>
       </c>
       <c r="C120" s="1">
-        <v>36</v>
+        <v>160</v>
       </c>
       <c r="D120" s="1">
         <v>0</v>
@@ -12973,7 +12973,7 @@
         <v>229</v>
       </c>
       <c r="C121" s="1">
-        <v>60</v>
+        <v>170</v>
       </c>
       <c r="D121" s="1">
         <v>0</v>
@@ -13015,7 +13015,7 @@
         <v>235</v>
       </c>
       <c r="C124" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D124" s="1">
         <v>0</v>
@@ -13029,7 +13029,7 @@
         <v>237</v>
       </c>
       <c r="C125" s="1">
-        <v>324</v>
+        <v>290</v>
       </c>
       <c r="D125" s="1">
         <v>0</v>
@@ -13211,7 +13211,7 @@
         <v>263</v>
       </c>
       <c r="C138" s="1">
-        <v>164</v>
+        <v>149</v>
       </c>
       <c r="D138" s="1">
         <v>0</v>
@@ -13308,7 +13308,7 @@
         <v>0</v>
       </c>
       <c r="D145" s="1">
-        <v>286</v>
+        <v>254</v>
       </c>
     </row>
     <row r="146" spans="1:4">
@@ -13565,7 +13565,7 @@
         <v>295</v>
       </c>
       <c r="C167" s="8">
-        <v>187</v>
+        <v>180</v>
       </c>
       <c r="D167" s="8">
         <v>0</v>
@@ -13593,7 +13593,7 @@
         <v>299</v>
       </c>
       <c r="C169" s="8">
-        <v>138</v>
+        <v>112</v>
       </c>
       <c r="D169" s="8">
         <v>0</v>
@@ -13607,7 +13607,7 @@
         <v>301</v>
       </c>
       <c r="C170" s="8">
-        <v>611</v>
+        <v>597</v>
       </c>
       <c r="D170" s="8">
         <v>0</v>
@@ -13621,7 +13621,7 @@
         <v>303</v>
       </c>
       <c r="C171" s="8">
-        <v>0</v>
+        <v>567</v>
       </c>
       <c r="D171" s="8">
         <v>0</v>
@@ -13635,7 +13635,7 @@
         <v>305</v>
       </c>
       <c r="C172" s="8">
-        <v>0</v>
+        <v>464</v>
       </c>
       <c r="D172" s="8">
         <v>0</v>
@@ -13649,7 +13649,7 @@
         <v>307</v>
       </c>
       <c r="C173" s="8">
-        <v>562</v>
+        <v>557</v>
       </c>
       <c r="D173" s="8">
         <v>0</v>
@@ -13663,7 +13663,7 @@
         <v>309</v>
       </c>
       <c r="C174" s="8">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D174" s="8">
         <v>0</v>
@@ -13719,7 +13719,7 @@
         <v>317</v>
       </c>
       <c r="C178" s="8">
-        <v>587</v>
+        <v>565</v>
       </c>
       <c r="D178" s="8">
         <v>0</v>
@@ -13733,7 +13733,7 @@
         <v>319</v>
       </c>
       <c r="C179" s="8">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="D179" s="8">
         <v>0</v>
@@ -13747,7 +13747,7 @@
         <v>321</v>
       </c>
       <c r="C180" s="8">
-        <v>392</v>
+        <v>389</v>
       </c>
       <c r="D180" s="8">
         <v>0</v>
@@ -13761,7 +13761,7 @@
         <v>323</v>
       </c>
       <c r="C181" s="8">
-        <v>215</v>
+        <v>75</v>
       </c>
       <c r="D181" s="8">
         <v>0</v>
@@ -13775,7 +13775,7 @@
         <v>325</v>
       </c>
       <c r="C182" s="8">
-        <v>426</v>
+        <v>420</v>
       </c>
       <c r="D182" s="8">
         <v>0</v>
@@ -13789,7 +13789,7 @@
         <v>327</v>
       </c>
       <c r="C183" s="8">
-        <v>0</v>
+        <v>41</v>
       </c>
       <c r="D183" s="8">
         <v>0</v>
@@ -13803,7 +13803,7 @@
         <v>329</v>
       </c>
       <c r="C184" s="9">
-        <v>2167</v>
+        <v>2142</v>
       </c>
       <c r="D184" s="8">
         <v>0</v>
@@ -13817,7 +13817,7 @@
         <v>331</v>
       </c>
       <c r="C185" s="8">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D185" s="8">
         <v>0</v>
@@ -13859,7 +13859,7 @@
         <v>337</v>
       </c>
       <c r="C188" s="8">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D188" s="8">
         <v>0</v>
@@ -13873,7 +13873,7 @@
         <v>339</v>
       </c>
       <c r="C189" s="8">
-        <v>80</v>
+        <v>39</v>
       </c>
       <c r="D189" s="8">
         <v>0</v>
@@ -13901,7 +13901,7 @@
         <v>343</v>
       </c>
       <c r="C191" s="8">
-        <v>124</v>
+        <v>96</v>
       </c>
       <c r="D191" s="8">
         <v>0</v>
@@ -13915,7 +13915,7 @@
         <v>345</v>
       </c>
       <c r="C192" s="8">
-        <v>391</v>
+        <v>379</v>
       </c>
       <c r="D192" s="8">
         <v>0</v>
@@ -13929,7 +13929,7 @@
         <v>347</v>
       </c>
       <c r="C193" s="8">
-        <v>135</v>
+        <v>127</v>
       </c>
       <c r="D193" s="8">
         <v>0</v>
@@ -13957,7 +13957,7 @@
         <v>351</v>
       </c>
       <c r="C195" s="8">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="D195" s="8">
         <v>0</v>
@@ -13985,7 +13985,7 @@
         <v>355</v>
       </c>
       <c r="C197" s="8">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="D197" s="8">
         <v>0</v>
@@ -14013,7 +14013,7 @@
         <v>359</v>
       </c>
       <c r="C199" s="8">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D199" s="8">
         <v>0</v>
@@ -14027,7 +14027,7 @@
         <v>361</v>
       </c>
       <c r="C200" s="8">
-        <v>624</v>
+        <v>614</v>
       </c>
       <c r="D200" s="8">
         <v>0</v>
@@ -14041,7 +14041,7 @@
         <v>363</v>
       </c>
       <c r="C201" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D201" s="1">
         <v>0</v>
@@ -14058,7 +14058,7 @@
         <v>238</v>
       </c>
       <c r="D202" s="1">
-        <v>456</v>
+        <v>310</v>
       </c>
     </row>
     <row r="203" spans="1:4">
@@ -14071,8 +14071,8 @@
       <c r="C203" s="1">
         <v>235</v>
       </c>
-      <c r="D203" s="1">
-        <v>935</v>
+      <c r="D203" s="5">
+        <v>1795</v>
       </c>
     </row>
     <row r="204" spans="1:4">
@@ -14282,7 +14282,7 @@
         <v>0</v>
       </c>
       <c r="D218" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="219" spans="1:4">
@@ -14352,7 +14352,7 @@
         <v>1</v>
       </c>
       <c r="D223" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="224" spans="1:4">
@@ -14478,7 +14478,7 @@
         <v>7</v>
       </c>
       <c r="D232" s="1">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="233" spans="1:4">
@@ -14797,7 +14797,7 @@
         <v>471</v>
       </c>
       <c r="C255" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D255" s="1">
         <v>0</v>
@@ -14811,7 +14811,7 @@
         <v>473</v>
       </c>
       <c r="C256" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D256" s="1">
         <v>0</v>
@@ -14895,7 +14895,7 @@
         <v>485</v>
       </c>
       <c r="C262" s="1">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="D262" s="1">
         <v>0</v>
@@ -14923,7 +14923,7 @@
         <v>489</v>
       </c>
       <c r="C264" s="1">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D264" s="1">
         <v>0</v>
@@ -15217,7 +15217,7 @@
         <v>531</v>
       </c>
       <c r="C285" s="1">
-        <v>151</v>
+        <v>124</v>
       </c>
       <c r="D285" s="1">
         <v>0</v>
@@ -15777,7 +15777,7 @@
         <v>611</v>
       </c>
       <c r="C325" s="1">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D325" s="1">
         <v>0</v>
@@ -15819,7 +15819,7 @@
         <v>617</v>
       </c>
       <c r="C328" s="1">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D328" s="1">
         <v>0</v>
@@ -16127,7 +16127,7 @@
         <v>661</v>
       </c>
       <c r="C350" s="1">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D350" s="1">
         <v>0</v>
@@ -16169,7 +16169,7 @@
         <v>667</v>
       </c>
       <c r="C353" s="1">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="D353" s="1">
         <v>0</v>
@@ -16211,7 +16211,7 @@
         <v>673</v>
       </c>
       <c r="C356" s="1">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="D356" s="1">
         <v>0</v>
@@ -16225,7 +16225,7 @@
         <v>675</v>
       </c>
       <c r="C357" s="1">
-        <v>16</v>
+        <v>38</v>
       </c>
       <c r="D357" s="1">
         <v>0</v>
@@ -16239,7 +16239,7 @@
         <v>677</v>
       </c>
       <c r="C358" s="1">
-        <v>-4</v>
+        <v>1</v>
       </c>
       <c r="D358" s="1">
         <v>0</v>
@@ -16253,7 +16253,7 @@
         <v>679</v>
       </c>
       <c r="C359" s="1">
-        <v>459</v>
+        <v>421</v>
       </c>
       <c r="D359" s="1">
         <v>0</v>
@@ -16267,7 +16267,7 @@
         <v>681</v>
       </c>
       <c r="C360" s="1">
-        <v>182</v>
+        <v>157</v>
       </c>
       <c r="D360" s="1">
         <v>0</v>
@@ -16281,7 +16281,7 @@
         <v>683</v>
       </c>
       <c r="C361" s="1">
-        <v>126</v>
+        <v>113</v>
       </c>
       <c r="D361" s="1">
         <v>0</v>
@@ -16295,7 +16295,7 @@
         <v>685</v>
       </c>
       <c r="C362" s="1">
-        <v>736</v>
+        <v>640</v>
       </c>
       <c r="D362" s="1">
         <v>0</v>
@@ -16309,7 +16309,7 @@
         <v>687</v>
       </c>
       <c r="C363" s="1">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="D363" s="1">
         <v>0</v>
@@ -16337,7 +16337,7 @@
         <v>691</v>
       </c>
       <c r="C365" s="1">
-        <v>131</v>
+        <v>110</v>
       </c>
       <c r="D365" s="1">
         <v>0</v>
@@ -16407,7 +16407,7 @@
         <v>701</v>
       </c>
       <c r="C370" s="1">
-        <v>7</v>
+        <v>29</v>
       </c>
       <c r="D370" s="1">
         <v>0</v>
@@ -16449,7 +16449,7 @@
         <v>707</v>
       </c>
       <c r="C373" s="1">
-        <v>1</v>
+        <v>49</v>
       </c>
       <c r="D373" s="1">
         <v>0</v>
@@ -16491,7 +16491,7 @@
         <v>713</v>
       </c>
       <c r="C376" s="1">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D376" s="1">
         <v>0</v>
@@ -16561,7 +16561,7 @@
         <v>723</v>
       </c>
       <c r="C381" s="1">
-        <v>74</v>
+        <v>57</v>
       </c>
       <c r="D381" s="1">
         <v>0</v>
@@ -16617,7 +16617,7 @@
         <v>731</v>
       </c>
       <c r="C385" s="1">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="D385" s="1">
         <v>0</v>
@@ -16631,7 +16631,7 @@
         <v>733</v>
       </c>
       <c r="C386" s="1">
-        <v>11</v>
+        <v>30</v>
       </c>
       <c r="D386" s="1">
         <v>0</v>
@@ -16645,7 +16645,7 @@
         <v>735</v>
       </c>
       <c r="C387" s="1">
-        <v>39</v>
+        <v>19</v>
       </c>
       <c r="D387" s="1">
         <v>0</v>
@@ -16659,7 +16659,7 @@
         <v>737</v>
       </c>
       <c r="C388" s="1">
-        <v>15</v>
+        <v>49</v>
       </c>
       <c r="D388" s="1">
         <v>0</v>
@@ -16673,7 +16673,7 @@
         <v>739</v>
       </c>
       <c r="C389" s="1">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D389" s="1">
         <v>0</v>
@@ -16687,7 +16687,7 @@
         <v>741</v>
       </c>
       <c r="C390" s="1">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D390" s="1">
         <v>0</v>
@@ -16715,7 +16715,7 @@
         <v>745</v>
       </c>
       <c r="C392" s="1">
-        <v>23</v>
+        <v>0</v>
       </c>
       <c r="D392" s="1">
         <v>0</v>
@@ -16743,7 +16743,7 @@
         <v>749</v>
       </c>
       <c r="C394" s="1">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="D394" s="1">
         <v>0</v>
@@ -16771,7 +16771,7 @@
         <v>753</v>
       </c>
       <c r="C396" s="1">
-        <v>40</v>
+        <v>-5</v>
       </c>
       <c r="D396" s="1">
         <v>0</v>
@@ -17331,7 +17331,7 @@
         <v>833</v>
       </c>
       <c r="C436" s="1">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="D436" s="1">
         <v>0</v>
@@ -17387,7 +17387,7 @@
         <v>841</v>
       </c>
       <c r="C440" s="1">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D440" s="1">
         <v>0</v>
@@ -17471,7 +17471,7 @@
         <v>853</v>
       </c>
       <c r="C446" s="1">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="D446" s="1">
         <v>0</v>
@@ -17513,7 +17513,7 @@
         <v>859</v>
       </c>
       <c r="C449" s="1">
-        <v>167</v>
+        <v>142</v>
       </c>
       <c r="D449" s="1">
         <v>0</v>
@@ -17569,7 +17569,7 @@
         <v>867</v>
       </c>
       <c r="C453" s="1">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="D453" s="1">
         <v>0</v>
@@ -17611,7 +17611,7 @@
         <v>873</v>
       </c>
       <c r="C456" s="1">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="D456" s="1">
         <v>0</v>
@@ -17667,7 +17667,7 @@
         <v>881</v>
       </c>
       <c r="C460" s="1">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D460" s="1">
         <v>0</v>
@@ -17723,7 +17723,7 @@
         <v>889</v>
       </c>
       <c r="C464" s="1">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="D464" s="1">
         <v>0</v>
@@ -17751,7 +17751,7 @@
         <v>893</v>
       </c>
       <c r="C466" s="1">
-        <v>79</v>
+        <v>66</v>
       </c>
       <c r="D466" s="1">
         <v>0</v>
@@ -17793,7 +17793,7 @@
         <v>899</v>
       </c>
       <c r="C469" s="1">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="D469" s="1">
         <v>0</v>
@@ -17821,7 +17821,7 @@
         <v>903</v>
       </c>
       <c r="C471" s="1">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D471" s="1">
         <v>0</v>
@@ -17863,7 +17863,7 @@
         <v>909</v>
       </c>
       <c r="C474" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D474" s="1">
         <v>0</v>
@@ -17891,7 +17891,7 @@
         <v>913</v>
       </c>
       <c r="C476" s="1">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D476" s="1">
         <v>0</v>
@@ -17933,7 +17933,7 @@
         <v>919</v>
       </c>
       <c r="C479" s="1">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D479" s="1">
         <v>0</v>
@@ -17961,7 +17961,7 @@
         <v>923</v>
       </c>
       <c r="C481" s="1">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D481" s="1">
         <v>0</v>
@@ -17975,7 +17975,7 @@
         <v>925</v>
       </c>
       <c r="C482" s="1">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D482" s="1">
         <v>0</v>
@@ -17989,7 +17989,7 @@
         <v>927</v>
       </c>
       <c r="C483" s="1">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="D483" s="1">
         <v>0</v>
@@ -18031,7 +18031,7 @@
         <v>933</v>
       </c>
       <c r="C486" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D486" s="1">
         <v>0</v>
@@ -18370,7 +18370,7 @@
         <v>48</v>
       </c>
       <c r="D510" s="1">
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
     <row r="511" spans="1:4">
@@ -18493,7 +18493,7 @@
         <v>999</v>
       </c>
       <c r="C519" s="1">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D519" s="1">
         <v>0</v>
@@ -18535,7 +18535,7 @@
         <v>1005</v>
       </c>
       <c r="C522" s="1">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D522" s="1">
         <v>0</v>
@@ -18675,7 +18675,7 @@
         <v>1025</v>
       </c>
       <c r="C532" s="1">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="D532" s="1">
         <v>0</v>
@@ -18745,10 +18745,10 @@
         <v>1035</v>
       </c>
       <c r="C537" s="1">
-        <v>5</v>
+        <v>109</v>
       </c>
       <c r="D537" s="1">
-        <v>465</v>
+        <v>441</v>
       </c>
     </row>
     <row r="538" spans="1:4">
@@ -18843,7 +18843,7 @@
         <v>1049</v>
       </c>
       <c r="C544" s="1">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D544" s="1">
         <v>0</v>
@@ -18871,7 +18871,7 @@
         <v>1053</v>
       </c>
       <c r="C546" s="1">
-        <v>99</v>
+        <v>84</v>
       </c>
       <c r="D546" s="1">
         <v>0</v>
@@ -18927,7 +18927,7 @@
         <v>1061</v>
       </c>
       <c r="C550" s="1">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="D550" s="1">
         <v>0</v>
@@ -18941,7 +18941,7 @@
         <v>1063</v>
       </c>
       <c r="C551" s="1">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="D551" s="1">
         <v>0</v>
@@ -19123,7 +19123,7 @@
         <v>1089</v>
       </c>
       <c r="C564" s="1">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D564" s="1">
         <v>0</v>
@@ -19235,7 +19235,7 @@
         <v>1105</v>
       </c>
       <c r="C572" s="1">
-        <v>-8</v>
+        <v>-4</v>
       </c>
       <c r="D572" s="1">
         <v>0</v>
@@ -19249,7 +19249,7 @@
         <v>1107</v>
       </c>
       <c r="C573" s="1">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D573" s="1">
         <v>0</v>
@@ -19375,7 +19375,7 @@
         <v>1125</v>
       </c>
       <c r="C582" s="1">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="D582" s="1">
         <v>0</v>
@@ -19389,7 +19389,7 @@
         <v>1127</v>
       </c>
       <c r="C583" s="1">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D583" s="1">
         <v>0</v>
@@ -19417,7 +19417,7 @@
         <v>1131</v>
       </c>
       <c r="C585" s="1">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="D585" s="1">
         <v>0</v>
@@ -19543,7 +19543,7 @@
         <v>1149</v>
       </c>
       <c r="C594" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D594" s="1">
         <v>0</v>
@@ -19599,7 +19599,7 @@
         <v>1157</v>
       </c>
       <c r="C598" s="1">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="D598" s="1">
         <v>0</v>
@@ -19655,7 +19655,7 @@
         <v>1165</v>
       </c>
       <c r="C602" s="1">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="D602" s="1">
         <v>0</v>
@@ -19725,7 +19725,7 @@
         <v>1175</v>
       </c>
       <c r="C607" s="1">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="D607" s="1">
         <v>0</v>
@@ -19781,7 +19781,7 @@
         <v>1183</v>
       </c>
       <c r="C611" s="1">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D611" s="1">
         <v>0</v>
@@ -19907,7 +19907,7 @@
         <v>1201</v>
       </c>
       <c r="C620" s="1">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D620" s="1">
         <v>0</v>
@@ -20103,7 +20103,7 @@
         <v>1229</v>
       </c>
       <c r="C634" s="1">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D634" s="1">
         <v>0</v>
@@ -20229,7 +20229,7 @@
         <v>1247</v>
       </c>
       <c r="C643" s="1">
-        <v>0</v>
+        <v>-3</v>
       </c>
       <c r="D643" s="1">
         <v>0</v>
@@ -20285,7 +20285,7 @@
         <v>1255</v>
       </c>
       <c r="C647" s="1">
-        <v>21</v>
+        <v>5</v>
       </c>
       <c r="D647" s="1">
         <v>0</v>
@@ -20341,7 +20341,7 @@
         <v>1263</v>
       </c>
       <c r="C651" s="1">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="D651" s="1">
         <v>0</v>
@@ -20439,7 +20439,7 @@
         <v>1277</v>
       </c>
       <c r="C658" s="1">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="D658" s="1">
         <v>0</v>
@@ -20635,7 +20635,7 @@
         <v>1305</v>
       </c>
       <c r="C672" s="1">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="D672" s="1">
         <v>0</v>
@@ -20859,7 +20859,7 @@
         <v>1337</v>
       </c>
       <c r="C688" s="1">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="D688" s="1">
         <v>0</v>
@@ -20929,7 +20929,7 @@
         <v>1347</v>
       </c>
       <c r="C693" s="1">
-        <v>403</v>
+        <v>343</v>
       </c>
       <c r="D693" s="1">
         <v>1</v>
@@ -20999,7 +20999,7 @@
         <v>1357</v>
       </c>
       <c r="C698" s="1">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D698" s="1">
         <v>0</v>
@@ -21055,7 +21055,7 @@
         <v>1365</v>
       </c>
       <c r="C702" s="1">
-        <v>44</v>
+        <v>73</v>
       </c>
       <c r="D702" s="1">
         <v>0</v>
@@ -21083,7 +21083,7 @@
         <v>1369</v>
       </c>
       <c r="C704" s="1">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D704" s="1">
         <v>0</v>
@@ -21181,7 +21181,7 @@
         <v>1383</v>
       </c>
       <c r="C711" s="1">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D711" s="1">
         <v>0</v>
@@ -21195,7 +21195,7 @@
         <v>1385</v>
       </c>
       <c r="C712" s="1">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="D712" s="1">
         <v>0</v>
@@ -21419,7 +21419,7 @@
         <v>1417</v>
       </c>
       <c r="C728" s="1">
-        <v>437</v>
+        <v>413</v>
       </c>
       <c r="D728" s="1">
         <v>0</v>
@@ -21545,7 +21545,7 @@
         <v>1435</v>
       </c>
       <c r="C737" s="1">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="D737" s="1">
         <v>0</v>
@@ -21671,7 +21671,7 @@
         <v>1453</v>
       </c>
       <c r="C746" s="1">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="D746" s="1">
         <v>0</v>
@@ -21685,7 +21685,7 @@
         <v>1455</v>
       </c>
       <c r="C747" s="1">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D747" s="1">
         <v>0</v>
@@ -21727,7 +21727,7 @@
         <v>1461</v>
       </c>
       <c r="C750" s="1">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D750" s="1">
         <v>0</v>
@@ -21797,7 +21797,7 @@
         <v>1471</v>
       </c>
       <c r="C755" s="1">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D755" s="1">
         <v>0</v>
@@ -21828,7 +21828,7 @@
         <v>0</v>
       </c>
       <c r="D757" s="1">
-        <v>-47</v>
+        <v>-108</v>
       </c>
     </row>
     <row r="758" spans="1:4">
@@ -22035,7 +22035,7 @@
         <v>1505</v>
       </c>
       <c r="C772" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D772" s="1">
         <v>0</v>
@@ -22049,7 +22049,7 @@
         <v>1507</v>
       </c>
       <c r="C773" s="1">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D773" s="1">
         <v>0</v>
@@ -22147,7 +22147,7 @@
         <v>1521</v>
       </c>
       <c r="C780" s="1">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="D780" s="1">
         <v>0</v>
@@ -22707,7 +22707,7 @@
         <v>1601</v>
       </c>
       <c r="C820" s="1">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D820" s="1">
         <v>0</v>
@@ -22735,7 +22735,7 @@
         <v>1605</v>
       </c>
       <c r="C822" s="1">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="D822" s="1">
         <v>0</v>
@@ -22777,7 +22777,7 @@
         <v>1611</v>
       </c>
       <c r="C825" s="1">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="D825" s="1">
         <v>0</v>
@@ -22833,10 +22833,10 @@
         <v>1619</v>
       </c>
       <c r="C829" s="1">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D829" s="1">
-        <v>60</v>
+        <v>51</v>
       </c>
     </row>
     <row r="830" spans="1:4">
@@ -22850,7 +22850,7 @@
         <v>0</v>
       </c>
       <c r="D830" s="1">
-        <v>45</v>
+        <v>35</v>
       </c>
     </row>
     <row r="831" spans="1:4">
@@ -22934,7 +22934,7 @@
         <v>0</v>
       </c>
       <c r="D836" s="1">
-        <v>13</v>
+        <v>6</v>
       </c>
     </row>
     <row r="837" spans="1:4">
@@ -22976,7 +22976,7 @@
         <v>0</v>
       </c>
       <c r="D839" s="1">
-        <v>13</v>
+        <v>4</v>
       </c>
     </row>
     <row r="840" spans="1:4">
@@ -23004,7 +23004,7 @@
         <v>0</v>
       </c>
       <c r="D841" s="1">
-        <v>18</v>
+        <v>2</v>
       </c>
     </row>
     <row r="842" spans="1:4">
@@ -23099,7 +23099,7 @@
         <v>1657</v>
       </c>
       <c r="C848" s="1">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D848" s="1">
         <v>0</v>
@@ -23127,7 +23127,7 @@
         <v>1661</v>
       </c>
       <c r="C850" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D850" s="1">
         <v>0</v>
@@ -23211,7 +23211,7 @@
         <v>1673</v>
       </c>
       <c r="C856" s="1">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D856" s="1">
         <v>0</v>
@@ -23561,7 +23561,7 @@
         <v>1723</v>
       </c>
       <c r="C881" s="1">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D881" s="1">
         <v>0</v>
@@ -24023,7 +24023,7 @@
         <v>1789</v>
       </c>
       <c r="C914" s="1">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="D914" s="1">
         <v>45</v>
@@ -24037,7 +24037,7 @@
         <v>1791</v>
       </c>
       <c r="C915" s="1">
-        <v>28</v>
+        <v>0</v>
       </c>
       <c r="D915" s="1">
         <v>0</v>
@@ -24079,7 +24079,7 @@
         <v>1797</v>
       </c>
       <c r="C918" s="1">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D918" s="1">
         <v>0</v>
@@ -24121,7 +24121,7 @@
         <v>1803</v>
       </c>
       <c r="C921" s="1">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="D921" s="1">
         <v>0</v>
@@ -24177,7 +24177,7 @@
         <v>1811</v>
       </c>
       <c r="C925" s="1">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="D925" s="1">
         <v>1</v>
@@ -24233,7 +24233,7 @@
         <v>1819</v>
       </c>
       <c r="C929" s="1">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D929" s="1">
         <v>0</v>
@@ -24303,7 +24303,7 @@
         <v>1829</v>
       </c>
       <c r="C934" s="1">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="D934" s="1">
         <v>0</v>
@@ -24317,7 +24317,7 @@
         <v>1831</v>
       </c>
       <c r="C935" s="1">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D935" s="1">
         <v>0</v>
@@ -24471,7 +24471,7 @@
         <v>1853</v>
       </c>
       <c r="C946" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D946" s="1">
         <v>0</v>
@@ -25073,7 +25073,7 @@
         <v>1939</v>
       </c>
       <c r="C989" s="1">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="D989" s="1">
         <v>0</v>
@@ -25087,7 +25087,7 @@
         <v>1941</v>
       </c>
       <c r="C990" s="1">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D990" s="1">
         <v>0</v>
@@ -25311,7 +25311,7 @@
         <v>1973</v>
       </c>
       <c r="C1006" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D1006" s="1">
         <v>0</v>
@@ -25381,7 +25381,7 @@
         <v>1983</v>
       </c>
       <c r="C1011" s="1">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="D1011" s="1">
         <v>0</v>
@@ -25451,7 +25451,7 @@
         <v>1993</v>
       </c>
       <c r="C1016" s="1">
-        <v>2</v>
+        <v>22</v>
       </c>
       <c r="D1016" s="1">
         <v>0</v>
@@ -25479,7 +25479,7 @@
         <v>1997</v>
       </c>
       <c r="C1018" s="1">
-        <v>0</v>
+        <v>82</v>
       </c>
       <c r="D1018" s="1">
         <v>0</v>
@@ -25493,7 +25493,7 @@
         <v>1999</v>
       </c>
       <c r="C1019" s="1">
-        <v>2</v>
+        <v>32</v>
       </c>
       <c r="D1019" s="1">
         <v>0</v>
@@ -25507,7 +25507,7 @@
         <v>2001</v>
       </c>
       <c r="C1020" s="1">
-        <v>1</v>
+        <v>49</v>
       </c>
       <c r="D1020" s="1">
         <v>0</v>
@@ -25521,7 +25521,7 @@
         <v>2003</v>
       </c>
       <c r="C1021" s="1">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="D1021" s="1">
         <v>0</v>
@@ -25549,7 +25549,7 @@
         <v>2007</v>
       </c>
       <c r="C1023" s="1">
-        <v>18</v>
+        <v>74</v>
       </c>
       <c r="D1023" s="1">
         <v>0</v>
@@ -25566,7 +25566,7 @@
         <v>0</v>
       </c>
       <c r="D1024" s="1">
-        <v>33</v>
+        <v>28</v>
       </c>
     </row>
     <row r="1025" spans="1:4">
@@ -25636,7 +25636,7 @@
         <v>0</v>
       </c>
       <c r="D1029" s="1">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="1030" spans="1:4">
@@ -25650,7 +25650,7 @@
         <v>0</v>
       </c>
       <c r="D1030" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1031" spans="1:4">
@@ -25692,7 +25692,7 @@
         <v>0</v>
       </c>
       <c r="D1033" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="1034" spans="1:4">
@@ -25706,7 +25706,7 @@
         <v>0</v>
       </c>
       <c r="D1034" s="1">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="1035" spans="1:4">
@@ -25720,7 +25720,7 @@
         <v>0</v>
       </c>
       <c r="D1035" s="1">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="1036" spans="1:4">
@@ -25734,7 +25734,7 @@
         <v>0</v>
       </c>
       <c r="D1036" s="1">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="1037" spans="1:4">
@@ -25748,7 +25748,7 @@
         <v>0</v>
       </c>
       <c r="D1037" s="1">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="1038" spans="1:4">
@@ -25762,7 +25762,7 @@
         <v>0</v>
       </c>
       <c r="D1038" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="1039" spans="1:4">
@@ -25804,7 +25804,7 @@
         <v>0</v>
       </c>
       <c r="D1041" s="1">
-        <v>8</v>
+        <v>11</v>
       </c>
     </row>
     <row r="1042" spans="1:4">
@@ -25818,7 +25818,7 @@
         <v>0</v>
       </c>
       <c r="D1042" s="1">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="1043" spans="1:4">
@@ -25874,7 +25874,7 @@
         <v>0</v>
       </c>
       <c r="D1046" s="1">
-        <v>-6</v>
+        <v>-12</v>
       </c>
     </row>
     <row r="1047" spans="1:4">
@@ -25888,7 +25888,7 @@
         <v>2</v>
       </c>
       <c r="D1047" s="1">
-        <v>26</v>
+        <v>6</v>
       </c>
     </row>
     <row r="1048" spans="1:4">
@@ -25916,7 +25916,7 @@
         <v>0</v>
       </c>
       <c r="D1049" s="1">
-        <v>47</v>
+        <v>41</v>
       </c>
     </row>
     <row r="1050" spans="1:4">
@@ -25930,7 +25930,7 @@
         <v>0</v>
       </c>
       <c r="D1050" s="1">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="1051" spans="1:4">
@@ -26277,7 +26277,7 @@
         <v>2111</v>
       </c>
       <c r="C1075" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D1075" s="1">
         <v>5</v>
@@ -26557,7 +26557,7 @@
         <v>2151</v>
       </c>
       <c r="C1095" s="1">
-        <v>224</v>
+        <v>207</v>
       </c>
       <c r="D1095" s="1">
         <v>0</v>
@@ -26627,7 +26627,7 @@
         <v>2161</v>
       </c>
       <c r="C1100" s="1">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D1100" s="1">
         <v>0</v>
@@ -26879,7 +26879,7 @@
         <v>2197</v>
       </c>
       <c r="C1118" s="1">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="D1118" s="1">
         <v>0</v>
@@ -26991,7 +26991,7 @@
         <v>2213</v>
       </c>
       <c r="C1126" s="1">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="D1126" s="1">
         <v>0</v>
@@ -27159,7 +27159,7 @@
         <v>2237</v>
       </c>
       <c r="C1138" s="1">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D1138" s="1">
         <v>0</v>
@@ -27285,7 +27285,7 @@
         <v>2255</v>
       </c>
       <c r="C1147" s="1">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D1147" s="1">
         <v>0</v>
@@ -27313,7 +27313,7 @@
         <v>2259</v>
       </c>
       <c r="C1149" s="1">
-        <v>183</v>
+        <v>147</v>
       </c>
       <c r="D1149" s="1">
         <v>0</v>
@@ -27397,7 +27397,7 @@
         <v>2271</v>
       </c>
       <c r="C1155" s="1">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="D1155" s="1">
         <v>0</v>
@@ -27607,7 +27607,7 @@
         <v>2301</v>
       </c>
       <c r="C1170" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D1170" s="1">
         <v>0</v>
@@ -27747,7 +27747,7 @@
         <v>2321</v>
       </c>
       <c r="C1180" s="1">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D1180" s="1">
         <v>0</v>
@@ -27775,7 +27775,7 @@
         <v>2325</v>
       </c>
       <c r="C1182" s="1">
-        <v>-89</v>
+        <v>-114</v>
       </c>
       <c r="D1182" s="1">
         <v>0</v>
@@ -27817,7 +27817,7 @@
         <v>2331</v>
       </c>
       <c r="C1185" s="1">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D1185" s="1">
         <v>0</v>
@@ -27845,7 +27845,7 @@
         <v>2335</v>
       </c>
       <c r="C1187" s="1">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D1187" s="1">
         <v>0</v>
@@ -27859,7 +27859,7 @@
         <v>2337</v>
       </c>
       <c r="C1188" s="1">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D1188" s="1">
         <v>0</v>
@@ -28335,7 +28335,7 @@
         <v>2405</v>
       </c>
       <c r="C1222" s="1">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="D1222" s="1">
         <v>0</v>
@@ -28391,7 +28391,7 @@
         <v>2413</v>
       </c>
       <c r="C1226" s="1">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="D1226" s="1">
         <v>0</v>
@@ -28615,7 +28615,7 @@
         <v>2445</v>
       </c>
       <c r="C1242" s="1">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D1242" s="1">
         <v>0</v>
@@ -28839,7 +28839,7 @@
         <v>2477</v>
       </c>
       <c r="C1258" s="1">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="D1258" s="1">
         <v>0</v>
@@ -29077,7 +29077,7 @@
         <v>2511</v>
       </c>
       <c r="C1275" s="1">
-        <v>4</v>
+        <v>22</v>
       </c>
       <c r="D1275" s="1">
         <v>0</v>
@@ -29203,7 +29203,7 @@
         <v>2529</v>
       </c>
       <c r="C1284" s="1">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D1284" s="1">
         <v>0</v>
@@ -29217,7 +29217,7 @@
         <v>2531</v>
       </c>
       <c r="C1285" s="1">
-        <v>131</v>
+        <v>123</v>
       </c>
       <c r="D1285" s="1">
         <v>0</v>
@@ -29245,7 +29245,7 @@
         <v>2535</v>
       </c>
       <c r="C1287" s="1">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D1287" s="1">
         <v>0</v>
@@ -29273,7 +29273,7 @@
         <v>2539</v>
       </c>
       <c r="C1289" s="1">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="D1289" s="1">
         <v>0</v>
@@ -30228,7 +30228,7 @@
         <v>0</v>
       </c>
       <c r="D1357" s="1">
-        <v>-35</v>
+        <v>-12</v>
       </c>
     </row>
     <row r="1358" spans="1:4">
@@ -30561,7 +30561,7 @@
         <v>2723</v>
       </c>
       <c r="C1381" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D1381" s="1">
         <v>0</v>
@@ -30687,7 +30687,7 @@
         <v>2741</v>
       </c>
       <c r="C1390" s="1">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D1390" s="1">
         <v>0</v>
@@ -30715,7 +30715,7 @@
         <v>2745</v>
       </c>
       <c r="C1392" s="1">
-        <v>45</v>
+        <v>24</v>
       </c>
       <c r="D1392" s="1">
         <v>0</v>
@@ -30729,7 +30729,7 @@
         <v>2747</v>
       </c>
       <c r="C1393" s="1">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D1393" s="1">
         <v>0</v>
@@ -31163,7 +31163,7 @@
         <v>2809</v>
       </c>
       <c r="C1424" s="1">
-        <v>5</v>
+        <v>69</v>
       </c>
       <c r="D1424" s="1">
         <v>0</v>
@@ -31275,7 +31275,7 @@
         <v>2825</v>
       </c>
       <c r="C1432" s="1">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D1432" s="1">
         <v>0</v>
@@ -31681,7 +31681,7 @@
         <v>2883</v>
       </c>
       <c r="C1461" s="1">
-        <v>5</v>
+        <v>-2</v>
       </c>
       <c r="D1461" s="1">
         <v>0</v>
@@ -31709,7 +31709,7 @@
         <v>2887</v>
       </c>
       <c r="C1463" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D1463" s="1">
         <v>0</v>
@@ -31779,7 +31779,7 @@
         <v>2897</v>
       </c>
       <c r="C1468" s="1">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="D1468" s="1">
         <v>0</v>
@@ -31835,7 +31835,7 @@
         <v>2905</v>
       </c>
       <c r="C1472" s="1">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D1472" s="1">
         <v>0</v>
@@ -31919,7 +31919,7 @@
         <v>2917</v>
       </c>
       <c r="C1478" s="1">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D1478" s="1">
         <v>0</v>
@@ -31933,7 +31933,7 @@
         <v>2919</v>
       </c>
       <c r="C1479" s="1">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="D1479" s="1">
         <v>0</v>
@@ -31961,7 +31961,7 @@
         <v>2923</v>
       </c>
       <c r="C1481" s="1">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="D1481" s="1">
         <v>0</v>
@@ -32129,7 +32129,7 @@
         <v>2947</v>
       </c>
       <c r="C1493" s="1">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D1493" s="1">
         <v>0</v>
@@ -32143,7 +32143,7 @@
         <v>2949</v>
       </c>
       <c r="C1494" s="1">
-        <v>904</v>
+        <v>888</v>
       </c>
       <c r="D1494" s="1">
         <v>0</v>
@@ -32563,7 +32563,7 @@
         <v>3009</v>
       </c>
       <c r="C1524" s="1">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D1524" s="1">
         <v>0</v>
@@ -32577,7 +32577,7 @@
         <v>3011</v>
       </c>
       <c r="C1525" s="1">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="D1525" s="1">
         <v>0</v>
@@ -33398,7 +33398,7 @@
         <v>0</v>
       </c>
       <c r="D1584" s="1">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="1585" spans="1:4">
@@ -33409,7 +33409,7 @@
         <v>3129</v>
       </c>
       <c r="C1585" s="1">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="D1585" s="1">
         <v>0</v>
@@ -33454,7 +33454,7 @@
         <v>3</v>
       </c>
       <c r="D1588" s="1">
-        <v>12</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1589" spans="1:4">
@@ -33521,7 +33521,7 @@
         <v>3145</v>
       </c>
       <c r="C1593" s="1">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D1593" s="1">
         <v>0</v>
@@ -33605,7 +33605,7 @@
         <v>3157</v>
       </c>
       <c r="C1599" s="1">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="D1599" s="1">
         <v>0</v>
@@ -33689,7 +33689,7 @@
         <v>3169</v>
       </c>
       <c r="C1605" s="1">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D1605" s="1">
         <v>0</v>
@@ -33703,7 +33703,7 @@
         <v>3171</v>
       </c>
       <c r="C1606" s="1">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D1606" s="1">
         <v>0</v>
@@ -33857,7 +33857,7 @@
         <v>3193</v>
       </c>
       <c r="C1617" s="1">
-        <v>39</v>
+        <v>1</v>
       </c>
       <c r="D1617" s="1">
         <v>0</v>
@@ -33913,7 +33913,7 @@
         <v>3201</v>
       </c>
       <c r="C1621" s="1">
-        <v>18</v>
+        <v>88</v>
       </c>
       <c r="D1621" s="1">
         <v>0</v>
@@ -33927,7 +33927,7 @@
         <v>3203</v>
       </c>
       <c r="C1622" s="1">
-        <v>48</v>
+        <v>34</v>
       </c>
       <c r="D1622" s="1">
         <v>0</v>
@@ -34067,7 +34067,7 @@
         <v>3223</v>
       </c>
       <c r="C1632" s="1">
-        <v>98</v>
+        <v>78</v>
       </c>
       <c r="D1632" s="1">
         <v>0</v>
@@ -34109,7 +34109,7 @@
         <v>3229</v>
       </c>
       <c r="C1635" s="1">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="D1635" s="1">
         <v>0</v>
@@ -34137,7 +34137,7 @@
         <v>3233</v>
       </c>
       <c r="C1637" s="1">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="D1637" s="1">
         <v>0</v>
@@ -34151,7 +34151,7 @@
         <v>3235</v>
       </c>
       <c r="C1638" s="1">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D1638" s="1">
         <v>0</v>
@@ -34193,7 +34193,7 @@
         <v>3241</v>
       </c>
       <c r="C1641" s="1">
-        <v>58</v>
+        <v>3</v>
       </c>
       <c r="D1641" s="1">
         <v>0</v>
@@ -34263,7 +34263,7 @@
         <v>3251</v>
       </c>
       <c r="C1646" s="1">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="D1646" s="1">
         <v>0</v>
@@ -34319,7 +34319,7 @@
         <v>3259</v>
       </c>
       <c r="C1650" s="1">
-        <v>0</v>
+        <v>-4</v>
       </c>
       <c r="D1650" s="1">
         <v>0</v>
@@ -34431,7 +34431,7 @@
         <v>3275</v>
       </c>
       <c r="C1658" s="1">
-        <v>203</v>
+        <v>192</v>
       </c>
       <c r="D1658" s="1">
         <v>0</v>
@@ -34445,7 +34445,7 @@
         <v>3277</v>
       </c>
       <c r="C1659" s="1">
-        <v>59</v>
+        <v>575</v>
       </c>
       <c r="D1659" s="1">
         <v>0</v>
@@ -34487,7 +34487,7 @@
         <v>3283</v>
       </c>
       <c r="C1662" s="1">
-        <v>207</v>
+        <v>463</v>
       </c>
       <c r="D1662" s="1">
         <v>0</v>
@@ -34529,7 +34529,7 @@
         <v>3289</v>
       </c>
       <c r="C1665" s="1">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="D1665" s="1">
         <v>0</v>
@@ -34879,7 +34879,7 @@
         <v>3339</v>
       </c>
       <c r="C1690" s="1">
-        <v>372</v>
+        <v>363</v>
       </c>
       <c r="D1690" s="1">
         <v>0</v>
@@ -35106,7 +35106,7 @@
         <v>0</v>
       </c>
       <c r="D1706" s="1">
-        <v>2</v>
+        <v>9</v>
       </c>
     </row>
     <row r="1707" spans="1:4">
@@ -35117,7 +35117,7 @@
         <v>3373</v>
       </c>
       <c r="C1707" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D1707" s="1">
         <v>0</v>
@@ -35131,7 +35131,7 @@
         <v>3375</v>
       </c>
       <c r="C1708" s="1">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="D1708" s="1">
         <v>0</v>
@@ -35145,7 +35145,7 @@
         <v>3377</v>
       </c>
       <c r="C1709" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D1709" s="1">
         <v>0</v>
@@ -35159,7 +35159,7 @@
         <v>3379</v>
       </c>
       <c r="C1710" s="1">
-        <v>8</v>
+        <v>69</v>
       </c>
       <c r="D1710" s="1">
         <v>0</v>
@@ -35173,7 +35173,7 @@
         <v>3381</v>
       </c>
       <c r="C1711" s="1">
-        <v>0</v>
+        <v>-8</v>
       </c>
       <c r="D1711" s="1">
         <v>0</v>
@@ -35190,7 +35190,7 @@
         <v>0</v>
       </c>
       <c r="D1712" s="1">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="1713" spans="1:4">
@@ -35201,7 +35201,7 @@
         <v>3385</v>
       </c>
       <c r="C1713" s="1">
-        <v>476</v>
+        <v>348</v>
       </c>
       <c r="D1713" s="1">
         <v>0</v>
@@ -35229,7 +35229,7 @@
         <v>3389</v>
       </c>
       <c r="C1715" s="5">
-        <v>6643</v>
+        <v>6544</v>
       </c>
       <c r="D1715" s="1">
         <v>0</v>
@@ -35243,7 +35243,7 @@
         <v>3391</v>
       </c>
       <c r="C1716" s="1">
-        <v>443</v>
+        <v>440</v>
       </c>
       <c r="D1716" s="1">
         <v>0</v>
@@ -35260,7 +35260,7 @@
         <v>0</v>
       </c>
       <c r="D1717" s="1">
-        <v>6</v>
+        <v>228</v>
       </c>
     </row>
     <row r="1718" spans="1:4">
@@ -35288,7 +35288,7 @@
         <v>0</v>
       </c>
       <c r="D1719" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1720" spans="1:4">
@@ -35439,7 +35439,7 @@
         <v>3419</v>
       </c>
       <c r="C1730" s="1">
-        <v>330</v>
+        <v>306</v>
       </c>
       <c r="D1730" s="1">
         <v>0</v>
@@ -35621,7 +35621,7 @@
         <v>3445</v>
       </c>
       <c r="C1743" s="1">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D1743" s="1">
         <v>0</v>
@@ -35691,7 +35691,7 @@
         <v>3455</v>
       </c>
       <c r="C1748" s="1">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D1748" s="1">
         <v>0</v>
@@ -35733,7 +35733,7 @@
         <v>3461</v>
       </c>
       <c r="C1751" s="1">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="D1751" s="1">
         <v>0</v>
@@ -35803,7 +35803,7 @@
         <v>3471</v>
       </c>
       <c r="C1756" s="1">
-        <v>19</v>
+        <v>-3</v>
       </c>
       <c r="D1756" s="1">
         <v>0</v>
@@ -35929,7 +35929,7 @@
         <v>3489</v>
       </c>
       <c r="C1765" s="1">
-        <v>174</v>
+        <v>165</v>
       </c>
       <c r="D1765" s="1">
         <v>0</v>
@@ -36083,7 +36083,7 @@
         <v>3511</v>
       </c>
       <c r="C1776" s="1">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="D1776" s="1">
         <v>0</v>
@@ -36251,7 +36251,7 @@
         <v>3535</v>
       </c>
       <c r="C1788" s="1">
-        <v>0</v>
+        <v>46</v>
       </c>
       <c r="D1788" s="1">
         <v>0</v>
@@ -36265,14 +36265,14 @@
         <v>3537</v>
       </c>
       <c r="C1789" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D1789" s="1">
         <v>0</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E1" xr:uid="{C837A1CC-3663-451F-A8FA-3F456AFF6EF2}"/>
+  <autoFilter ref="A1:E1789" xr:uid="{C837A1CC-3663-451F-A8FA-3F456AFF6EF2}"/>
   <phoneticPr fontId="7"/>
   <conditionalFormatting sqref="A1 A1790:A1048576">
     <cfRule type="duplicateValues" dxfId="0" priority="1"/>

</xml_diff>